<commit_message>
separated Start for testing, added report message to Mass_Balance_Cor
</commit_message>
<xml_diff>
--- a/docu/TestExperimentSet1/TestExperiment2.xlsx
+++ b/docu/TestExperimentSet1/TestExperiment2.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20387"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5522C90C-4D2D-4CE0-8703-0E82B5D31E92}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347392C2-4629-439A-A85D-3E27235084B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7260" yWindow="1515" windowWidth="16155" windowHeight="12510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -802,7 +802,7 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1082,8 +1082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10:J12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1382,7 +1382,7 @@
         <v>0</v>
       </c>
       <c r="E20" s="20">
-        <v>10277</v>
+        <v>10.276999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1399,7 +1399,7 @@
         <v>0</v>
       </c>
       <c r="E21" s="20">
-        <v>16449</v>
+        <v>16.449000000000002</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1416,7 +1416,7 @@
         <v>0</v>
       </c>
       <c r="E22" s="20">
-        <v>18823</v>
+        <v>18.823</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1433,7 +1433,7 @@
         <v>0</v>
       </c>
       <c r="E23" s="20">
-        <v>17966</v>
+        <v>17.966000000000001</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1450,7 +1450,7 @@
         <v>0</v>
       </c>
       <c r="E24" s="20">
-        <v>15729</v>
+        <v>15.728999999999999</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1467,7 +1467,7 @@
         <v>0</v>
       </c>
       <c r="E25" s="20">
-        <v>1281</v>
+        <v>1.2809999999999999</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>